<commit_message>
refactor test DDT + API
</commit_message>
<xml_diff>
--- a/External Resources/Business/Cupo/CasosPruebaValidarCupo.xlsx
+++ b/External Resources/Business/Cupo/CasosPruebaValidarCupo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio.olivieri\RobotTesting\YARD\External Resources\Business\Cupo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC2E293-74E6-41B4-AA30-7BBCD2DACC1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D5E517-2BAB-4E21-A79D-932DDD649063}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
   <si>
     <t>${IdFinalidad}</t>
   </si>
@@ -110,13 +110,67 @@
   </si>
   <si>
     <t>${IdChofer}</t>
+  </si>
+  <si>
+    <t>${Msj}</t>
+  </si>
+  <si>
+    <t>Tarjeta en uso</t>
+  </si>
+  <si>
+    <t>El formato y la longitud de los dígitos ingresados no corresponde con el Documento de Porte seleccionado</t>
+  </si>
+  <si>
+    <t>La Tarjeta no existe</t>
+  </si>
+  <si>
+    <t>LDC NO debe ser Titular CP, Vendedor y Destinatario para la Finalidad seleccionada.</t>
+  </si>
+  <si>
+    <t>El Destinatario debe ser LDC para la Finalidad seleccionada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El campo 'Producto' es requerido. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El campo 'Vendedor' es requerido. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El campo 'CorredorComprador' es requerido. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El campo 'Destinatario' es requerido. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El campo 'Finalidad' es requerido. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El campo 'MotivoCupo' es requerido. </t>
+  </si>
+  <si>
+    <t>Error con el CTG ingresado: 1) no coincide con la Carta de Porte ingresada, ó 2) ya fue anulado, ó 3) no existe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El número de Documento de Porte ya existe en el Sistema. </t>
+  </si>
+  <si>
+    <t>Para la finalidad Compra/Venta, LDC debe ser el destinatario.</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>PENDIENTE</t>
+  </si>
+  <si>
+    <t>prueba</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,8 +184,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +202,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -157,12 +224,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,198 +573,1378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W10" sqref="W10"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="87.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="M1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="AC1" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
         <v>51</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>7</v>
       </c>
-      <c r="E2" s="3">
-        <v>888811111135</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
+      <c r="E2" s="8"/>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
         <v>23</v>
       </c>
-      <c r="I2" s="2">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2">
-        <v>2</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2">
-        <v>1</v>
-      </c>
-      <c r="O2" s="2">
+      <c r="I2" s="1">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
         <v>40</v>
       </c>
-      <c r="R2" s="2">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0</v>
-      </c>
-      <c r="U2" s="2">
-        <v>77</v>
-      </c>
-      <c r="V2" s="2">
-        <v>1</v>
-      </c>
-      <c r="W2" s="4">
-        <v>0</v>
-      </c>
-      <c r="X2" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="4">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="4">
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="U2" s="4">
+        <v>8</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1</v>
+      </c>
+      <c r="W2" s="2">
+        <v>0</v>
+      </c>
+      <c r="X2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="2">
         <v>22</v>
       </c>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4">
-        <v>2</v>
+      <c r="AB2" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>51</v>
+      </c>
+      <c r="D3" s="2">
+        <v>7</v>
+      </c>
+      <c r="E3" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="1">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>40</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="4">
+        <v>8</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1</v>
+      </c>
+      <c r="W3" s="2">
+        <v>0</v>
+      </c>
+      <c r="X3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>51</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
+        <v>23</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="1">
+        <v>2</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>40</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="4">
+        <v>8</v>
+      </c>
+      <c r="V4" s="1">
+        <v>1</v>
+      </c>
+      <c r="W4" s="2">
+        <v>0</v>
+      </c>
+      <c r="X4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>51</v>
+      </c>
+      <c r="D5" s="2">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>23</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>40</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="4">
+        <v>8</v>
+      </c>
+      <c r="V5" s="1">
+        <v>1</v>
+      </c>
+      <c r="W5" s="2">
+        <v>0</v>
+      </c>
+      <c r="X5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>51</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>23</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2</v>
+      </c>
+      <c r="K6" s="6"/>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
+        <v>40</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="4">
+        <v>8</v>
+      </c>
+      <c r="V6" s="1">
+        <v>1</v>
+      </c>
+      <c r="W6" s="2">
+        <v>0</v>
+      </c>
+      <c r="X6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2">
+        <v>51</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7</v>
+      </c>
+      <c r="E7" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>23</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="M7" s="7"/>
+      <c r="N7" s="1">
+        <v>1</v>
+      </c>
+      <c r="O7" s="1">
+        <v>40</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="4">
+        <v>8</v>
+      </c>
+      <c r="V7" s="1">
+        <v>1</v>
+      </c>
+      <c r="W7" s="2">
+        <v>0</v>
+      </c>
+      <c r="X7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>51</v>
+      </c>
+      <c r="D8" s="2">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>23</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1">
+        <v>2</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7"/>
+      <c r="O8" s="1">
+        <v>40</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="U8" s="4">
+        <v>8</v>
+      </c>
+      <c r="V8" s="1">
+        <v>1</v>
+      </c>
+      <c r="W8" s="2">
+        <v>0</v>
+      </c>
+      <c r="X8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2">
+        <v>51</v>
+      </c>
+      <c r="D9" s="2">
+        <v>7</v>
+      </c>
+      <c r="E9" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>23</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1</v>
+      </c>
+      <c r="O9" s="1">
+        <v>40</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="U9" s="4">
+        <v>8</v>
+      </c>
+      <c r="V9" s="1">
+        <v>1</v>
+      </c>
+      <c r="W9" s="2">
+        <v>0</v>
+      </c>
+      <c r="X9" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC9" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>51</v>
+      </c>
+      <c r="D10" s="2">
+        <v>7</v>
+      </c>
+      <c r="E10" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
+        <v>23</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1">
+        <v>40</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="U10" s="4">
+        <v>8</v>
+      </c>
+      <c r="V10" s="1">
+        <v>1</v>
+      </c>
+      <c r="W10" s="2">
+        <v>1</v>
+      </c>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2">
+        <v>51</v>
+      </c>
+      <c r="D11" s="2">
+        <v>7</v>
+      </c>
+      <c r="E11" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>23</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1">
+        <v>40</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="U11" s="6"/>
+      <c r="V11" s="1">
+        <v>1</v>
+      </c>
+      <c r="W11" s="2">
+        <v>1</v>
+      </c>
+      <c r="X11" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2">
+        <v>51</v>
+      </c>
+      <c r="D12" s="2">
+        <v>7</v>
+      </c>
+      <c r="E12" s="8">
+        <v>888811111144</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <v>23</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>2</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1">
+        <v>1</v>
+      </c>
+      <c r="O12" s="1">
+        <v>40</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
+      <c r="U12" s="4">
+        <v>8</v>
+      </c>
+      <c r="V12" s="1">
+        <v>1</v>
+      </c>
+      <c r="W12" s="2">
+        <v>1</v>
+      </c>
+      <c r="X12" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2">
+        <v>51</v>
+      </c>
+      <c r="D13" s="2">
+        <v>7</v>
+      </c>
+      <c r="E13" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4">
+        <v>23</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1">
+        <v>40</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
+      <c r="U13" s="6">
+        <v>14</v>
+      </c>
+      <c r="V13" s="1">
+        <v>1</v>
+      </c>
+      <c r="W13" s="2">
+        <v>1</v>
+      </c>
+      <c r="X13" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2">
+        <v>51</v>
+      </c>
+      <c r="D14" s="2">
+        <v>7</v>
+      </c>
+      <c r="E14" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4">
+        <v>23</v>
+      </c>
+      <c r="I14" s="1">
+        <v>2</v>
+      </c>
+      <c r="J14" s="1">
+        <v>2</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="M14" s="4">
+        <v>6</v>
+      </c>
+      <c r="N14" s="4">
+        <v>4</v>
+      </c>
+      <c r="O14" s="1">
+        <v>40</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0</v>
+      </c>
+      <c r="S14" s="1">
+        <v>0</v>
+      </c>
+      <c r="U14" s="4">
+        <v>8</v>
+      </c>
+      <c r="V14" s="1">
+        <v>1</v>
+      </c>
+      <c r="W14" s="2">
+        <v>1</v>
+      </c>
+      <c r="X14" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2">
+        <v>51</v>
+      </c>
+      <c r="D15" s="2">
+        <v>7</v>
+      </c>
+      <c r="E15" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
+        <v>23</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2</v>
+      </c>
+      <c r="J15" s="1">
+        <v>2</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="M15" s="4">
+        <v>6</v>
+      </c>
+      <c r="N15" s="4">
+        <v>4</v>
+      </c>
+      <c r="O15" s="1">
+        <v>40</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0</v>
+      </c>
+      <c r="U15" s="4">
+        <v>8</v>
+      </c>
+      <c r="V15" s="1">
+        <v>1</v>
+      </c>
+      <c r="W15" s="2">
+        <v>1</v>
+      </c>
+      <c r="X15" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2">
+        <v>51</v>
+      </c>
+      <c r="D16" s="2">
+        <v>7</v>
+      </c>
+      <c r="E16" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4">
+        <v>23</v>
+      </c>
+      <c r="I16" s="7">
+        <v>1</v>
+      </c>
+      <c r="J16" s="7">
+        <v>1</v>
+      </c>
+      <c r="K16" s="7">
+        <v>2</v>
+      </c>
+      <c r="M16" s="6">
+        <v>1</v>
+      </c>
+      <c r="N16" s="4">
+        <v>1</v>
+      </c>
+      <c r="O16" s="1">
+        <v>40</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0</v>
+      </c>
+      <c r="U16" s="4">
+        <v>8</v>
+      </c>
+      <c r="V16" s="1">
+        <v>1</v>
+      </c>
+      <c r="W16" s="2">
+        <v>1</v>
+      </c>
+      <c r="X16" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2">
+        <v>51</v>
+      </c>
+      <c r="D17" s="2">
+        <v>7</v>
+      </c>
+      <c r="E17" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="4">
+        <v>23</v>
+      </c>
+      <c r="I17" s="7">
+        <v>1</v>
+      </c>
+      <c r="J17" s="7">
+        <v>1</v>
+      </c>
+      <c r="K17" s="7">
+        <v>2</v>
+      </c>
+      <c r="M17" s="6">
+        <v>3</v>
+      </c>
+      <c r="N17" s="4">
+        <v>6</v>
+      </c>
+      <c r="O17" s="1">
+        <v>40</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0</v>
+      </c>
+      <c r="U17" s="4">
+        <v>8</v>
+      </c>
+      <c r="V17" s="1">
+        <v>1</v>
+      </c>
+      <c r="W17" s="2">
+        <v>1</v>
+      </c>
+      <c r="X17" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="2">
+        <v>51</v>
+      </c>
+      <c r="D18" s="2">
+        <v>7</v>
+      </c>
+      <c r="E18" s="5">
+        <v>888811111152</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="9">
+        <v>23</v>
+      </c>
+      <c r="I18" s="1">
+        <v>2</v>
+      </c>
+      <c r="J18" s="1">
+        <v>2</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1</v>
+      </c>
+      <c r="N18" s="1">
+        <v>1</v>
+      </c>
+      <c r="O18" s="1">
+        <v>40</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0</v>
+      </c>
+      <c r="S18" s="1">
+        <v>0</v>
+      </c>
+      <c r="U18" s="4">
+        <v>8</v>
+      </c>
+      <c r="V18" s="1">
+        <v>1</v>
+      </c>
+      <c r="W18" s="2">
+        <v>1</v>
+      </c>
+      <c r="X18" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>22</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC18" s="2"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="4">
+        <v>51</v>
+      </c>
+      <c r="D19" s="4">
+        <v>7</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="O19" s="4">
+        <v>40</v>
+      </c>
+      <c r="R19" s="4">
+        <v>0</v>
+      </c>
+      <c r="S19" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="4">
+        <v>51</v>
+      </c>
+      <c r="D20" s="4">
+        <v>7</v>
+      </c>
+      <c r="E20" s="5">
+        <v>888811111153</v>
+      </c>
+      <c r="O20" s="4">
+        <v>40</v>
+      </c>
+      <c r="P20" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R20" s="4">
+        <v>0</v>
+      </c>
+      <c r="S20" s="4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>